<commit_message>
Beginnings of board GUI
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameBSJM\ourData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\CSCI306\ClueGameBSMSLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="33">
   <si>
     <t>A</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>MU</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>PN</t>
   </si>
 </sst>
 </file>
@@ -492,7 +519,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X1" activeCellId="1" sqref="W1:W1048576 X1:X1048576"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>0</v>
@@ -609,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>4</v>
@@ -727,7 +754,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>3</v>
@@ -1100,7 +1127,7 @@
         <v>21</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="T9" s="6" t="s">
         <v>5</v>
@@ -1253,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>1</v>
@@ -1366,7 +1393,7 @@
         <v>6</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="R13" s="6" t="s">
         <v>6</v>
@@ -1797,7 +1824,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>2</v>
@@ -1821,7 +1848,7 @@
         <v>8</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>8</v>
@@ -1981,7 +2008,7 @@
         <v>7</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="S22" s="6" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
minor display issues fixed.
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\CSCI306\ClueGameBSMSLP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Meg/Documents/Mines/16-17 S2/Software Engineering/ClueGameBSMSLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17580" windowHeight="14080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -128,7 +134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,7 +193,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -196,11 +202,11 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -209,7 +215,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -217,7 +223,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -518,16 +524,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="22" width="6.28515625" customWidth="1"/>
+    <col min="1" max="22" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -595,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -663,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -731,7 +737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -799,7 +805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -867,7 +873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
@@ -935,7 +941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
@@ -1003,7 +1009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
@@ -1275,7 +1281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
@@ -1615,7 +1621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
@@ -1683,7 +1689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>2</v>
       </c>
@@ -1751,7 +1757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>2</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>2</v>
       </c>
@@ -1887,7 +1893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>2</v>
       </c>
@@ -1955,7 +1961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>0</v>
       </c>

</xml_diff>